<commit_message>
power output is nu correct
</commit_message>
<xml_diff>
--- a/results/end_of_day_charge_levels.xlsx
+++ b/results/end_of_day_charge_levels.xlsx
@@ -470,7 +470,7 @@
         <v>36528</v>
       </c>
       <c r="B4" t="n">
-        <v>0.3958056328221246</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -478,7 +478,7 @@
         <v>36529</v>
       </c>
       <c r="B5" t="n">
-        <v>0.1613898885714336</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -486,7 +486,7 @@
         <v>36530</v>
       </c>
       <c r="B6" t="n">
-        <v>0.1087805048860725</v>
+        <v>0.06366381003880003</v>
       </c>
     </row>
     <row r="7">
@@ -510,7 +510,7 @@
         <v>36533</v>
       </c>
       <c r="B9" t="n">
-        <v>0.2714434994611216</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -566,7 +566,7 @@
         <v>36540</v>
       </c>
       <c r="B16" t="n">
-        <v>0.5575336893186641</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -678,7 +678,7 @@
         <v>36554</v>
       </c>
       <c r="B30" t="n">
-        <v>2.61961158957724</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -686,7 +686,7 @@
         <v>36555</v>
       </c>
       <c r="B31" t="n">
-        <v>4.131527751806126</v>
+        <v>3.588460746437567</v>
       </c>
     </row>
     <row r="32">
@@ -710,7 +710,7 @@
         <v>36558</v>
       </c>
       <c r="B34" t="n">
-        <v>0.3452882775978262</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -934,7 +934,7 @@
         <v>36587</v>
       </c>
       <c r="B62" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -1014,7 +1014,7 @@
         <v>36597</v>
       </c>
       <c r="B72" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73">
@@ -1022,7 +1022,7 @@
         <v>36598</v>
       </c>
       <c r="B73" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -1038,7 +1038,7 @@
         <v>36600</v>
       </c>
       <c r="B75" t="n">
-        <v>5</v>
+        <v>4.154078783986692</v>
       </c>
     </row>
     <row r="76">
@@ -1046,7 +1046,7 @@
         <v>36601</v>
       </c>
       <c r="B76" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -1062,7 +1062,7 @@
         <v>36603</v>
       </c>
       <c r="B78" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="79">
@@ -1070,7 +1070,7 @@
         <v>36604</v>
       </c>
       <c r="B79" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80">
@@ -1078,7 +1078,7 @@
         <v>36605</v>
       </c>
       <c r="B80" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -1086,7 +1086,7 @@
         <v>36606</v>
       </c>
       <c r="B81" t="n">
-        <v>1.825030703966957</v>
+        <v>4.999999999999998</v>
       </c>
     </row>
     <row r="82">
@@ -1094,7 +1094,7 @@
         <v>36607</v>
       </c>
       <c r="B82" t="n">
-        <v>1.765414291084767</v>
+        <v>3.243283972901243</v>
       </c>
     </row>
     <row r="83">
@@ -1102,7 +1102,7 @@
         <v>36608</v>
       </c>
       <c r="B83" t="n">
-        <v>4.480065492322488</v>
+        <v>3.326071396160306</v>
       </c>
     </row>
     <row r="84">
@@ -1110,7 +1110,7 @@
         <v>36609</v>
       </c>
       <c r="B84" t="n">
-        <v>2.967103423383127</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85">
@@ -1118,7 +1118,7 @@
         <v>36610</v>
       </c>
       <c r="B85" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86">
@@ -1142,7 +1142,7 @@
         <v>36613</v>
       </c>
       <c r="B88" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89">
@@ -1166,7 +1166,7 @@
         <v>36616</v>
       </c>
       <c r="B91" t="n">
-        <v>4.999999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92">
@@ -1174,7 +1174,7 @@
         <v>36617</v>
       </c>
       <c r="B92" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93">
@@ -1510,7 +1510,7 @@
         <v>36659</v>
       </c>
       <c r="B134" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135">
@@ -1662,7 +1662,7 @@
         <v>36678</v>
       </c>
       <c r="B153" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154">
@@ -1814,7 +1814,7 @@
         <v>36697</v>
       </c>
       <c r="B172" t="n">
-        <v>4.999999999999997</v>
+        <v>5</v>
       </c>
     </row>
     <row r="173">
@@ -1838,7 +1838,7 @@
         <v>36700</v>
       </c>
       <c r="B175" t="n">
-        <v>5</v>
+        <v>1.942000742333645</v>
       </c>
     </row>
     <row r="176">
@@ -1846,7 +1846,7 @@
         <v>36701</v>
       </c>
       <c r="B176" t="n">
-        <v>2.25849875401698</v>
+        <v>3.950490898271326</v>
       </c>
     </row>
     <row r="177">
@@ -1854,7 +1854,7 @@
         <v>36702</v>
       </c>
       <c r="B177" t="n">
-        <v>2.656930401660337</v>
+        <v>5</v>
       </c>
     </row>
     <row r="178">
@@ -1870,7 +1870,7 @@
         <v>36704</v>
       </c>
       <c r="B179" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="180">
@@ -1886,7 +1886,7 @@
         <v>36706</v>
       </c>
       <c r="B181" t="n">
-        <v>5</v>
+        <v>4.145487026351776</v>
       </c>
     </row>
     <row r="182">
@@ -1894,7 +1894,7 @@
         <v>36707</v>
       </c>
       <c r="B182" t="n">
-        <v>4.322434453010724</v>
+        <v>0.2922529296163545</v>
       </c>
     </row>
     <row r="183">
@@ -1902,7 +1902,7 @@
         <v>36708</v>
       </c>
       <c r="B183" t="n">
-        <v>0.284756352717739</v>
+        <v>5</v>
       </c>
     </row>
     <row r="184">
@@ -2566,7 +2566,7 @@
         <v>36791</v>
       </c>
       <c r="B266" t="n">
-        <v>5</v>
+        <v>4.596364078714711</v>
       </c>
     </row>
     <row r="267">
@@ -2574,7 +2574,7 @@
         <v>36792</v>
       </c>
       <c r="B267" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="268">
@@ -2582,7 +2582,7 @@
         <v>36793</v>
       </c>
       <c r="B268" t="n">
-        <v>5</v>
+        <v>4.999999999999998</v>
       </c>
     </row>
     <row r="269">
@@ -2822,7 +2822,7 @@
         <v>36823</v>
       </c>
       <c r="B298" t="n">
-        <v>0.8025730305407738</v>
+        <v>0.7132873572634397</v>
       </c>
     </row>
     <row r="299">
@@ -2830,7 +2830,7 @@
         <v>36824</v>
       </c>
       <c r="B299" t="n">
-        <v>4.356958194396624</v>
+        <v>0</v>
       </c>
     </row>
     <row r="300">
@@ -2870,7 +2870,7 @@
         <v>36829</v>
       </c>
       <c r="B304" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="305">
@@ -2878,7 +2878,7 @@
         <v>36830</v>
       </c>
       <c r="B305" t="n">
-        <v>2.595872217399236</v>
+        <v>2.454299652530172</v>
       </c>
     </row>
     <row r="306">
@@ -2886,7 +2886,7 @@
         <v>36831</v>
       </c>
       <c r="B306" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="307">
@@ -2982,7 +2982,7 @@
         <v>36843</v>
       </c>
       <c r="B318" t="n">
-        <v>4.116536420790202</v>
+        <v>3.115238810587208</v>
       </c>
     </row>
     <row r="319">
@@ -3030,7 +3030,7 @@
         <v>36849</v>
       </c>
       <c r="B324" t="n">
-        <v>1.144897312399812</v>
+        <v>0.6463981650075452</v>
       </c>
     </row>
     <row r="325">
@@ -3038,7 +3038,7 @@
         <v>36850</v>
       </c>
       <c r="B325" t="n">
-        <v>2.391055075323611</v>
+        <v>0</v>
       </c>
     </row>
     <row r="326">
@@ -3110,7 +3110,7 @@
         <v>36859</v>
       </c>
       <c r="B334" t="n">
-        <v>0.1558759839757466</v>
+        <v>0</v>
       </c>
     </row>
     <row r="335">
@@ -3126,7 +3126,7 @@
         <v>36861</v>
       </c>
       <c r="B336" t="n">
-        <v>0.6565391915428718</v>
+        <v>0.5056632075671252</v>
       </c>
     </row>
     <row r="337">
@@ -3134,7 +3134,7 @@
         <v>36862</v>
       </c>
       <c r="B337" t="n">
-        <v>0.5178220611193987</v>
+        <v>0</v>
       </c>
     </row>
     <row r="338">
@@ -3142,7 +3142,7 @@
         <v>36863</v>
       </c>
       <c r="B338" t="n">
-        <v>0.7884789668474173</v>
+        <v>0.3600015234434402</v>
       </c>
     </row>
     <row r="339">
@@ -3158,7 +3158,7 @@
         <v>36865</v>
       </c>
       <c r="B340" t="n">
-        <v>0.4326335060876109</v>
+        <v>0.392076332707383</v>
       </c>
     </row>
     <row r="341">
@@ -3166,7 +3166,7 @@
         <v>36866</v>
       </c>
       <c r="B341" t="n">
-        <v>0.0416462999228427</v>
+        <v>0</v>
       </c>
     </row>
     <row r="342">
@@ -3174,7 +3174,7 @@
         <v>36867</v>
       </c>
       <c r="B342" t="n">
-        <v>0.01564629992284271</v>
+        <v>0</v>
       </c>
     </row>
     <row r="343">
@@ -3182,7 +3182,7 @@
         <v>36868</v>
       </c>
       <c r="B343" t="n">
-        <v>0.04055717338022789</v>
+        <v>0</v>
       </c>
     </row>
     <row r="344">
@@ -3230,7 +3230,7 @@
         <v>36874</v>
       </c>
       <c r="B349" t="n">
-        <v>0.1637141875419651</v>
+        <v>0.001317988031008764</v>
       </c>
     </row>
     <row r="350">
@@ -3238,7 +3238,7 @@
         <v>36875</v>
       </c>
       <c r="B350" t="n">
-        <v>0.518119155094375</v>
+        <v>0.2894244325588191</v>
       </c>
     </row>
     <row r="351">
@@ -3270,7 +3270,7 @@
         <v>36879</v>
       </c>
       <c r="B354" t="n">
-        <v>0.1360172536034742</v>
+        <v>0</v>
       </c>
     </row>
     <row r="355">
@@ -3286,7 +3286,7 @@
         <v>36881</v>
       </c>
       <c r="B356" t="n">
-        <v>1.43252855873512</v>
+        <v>0</v>
       </c>
     </row>
     <row r="357">
@@ -3302,7 +3302,7 @@
         <v>36883</v>
       </c>
       <c r="B358" t="n">
-        <v>1.59652855873512</v>
+        <v>0</v>
       </c>
     </row>
     <row r="359">
@@ -3310,7 +3310,7 @@
         <v>36884</v>
       </c>
       <c r="B359" t="n">
-        <v>1.791000790364842</v>
+        <v>1.449449116031491</v>
       </c>
     </row>
     <row r="360">

</xml_diff>

<commit_message>
cleaned main and finished financial_evaluation (except values for investment_cost
</commit_message>
<xml_diff>
--- a/results/end_of_day_charge_levels.xlsx
+++ b/results/end_of_day_charge_levels.xlsx
@@ -454,7 +454,7 @@
         <v>36526</v>
       </c>
       <c r="B2" t="n">
-        <v>0.6612923584120469</v>
+        <v>0.6612923584120468</v>
       </c>
     </row>
     <row r="3">
@@ -550,7 +550,7 @@
         <v>36538</v>
       </c>
       <c r="B14" t="n">
-        <v>0.4147975016967798</v>
+        <v>0.4147975016967796</v>
       </c>
     </row>
     <row r="15">
@@ -582,7 +582,7 @@
         <v>36542</v>
       </c>
       <c r="B18" t="n">
-        <v>0.3017559711545988</v>
+        <v>0.3017559711545987</v>
       </c>
     </row>
     <row r="19">
@@ -590,7 +590,7 @@
         <v>36543</v>
       </c>
       <c r="B19" t="n">
-        <v>0.4618964675591821</v>
+        <v>0.461896467559182</v>
       </c>
     </row>
     <row r="20">
@@ -598,7 +598,7 @@
         <v>36544</v>
       </c>
       <c r="B20" t="n">
-        <v>2.85000523098653</v>
+        <v>2.850005230986529</v>
       </c>
     </row>
     <row r="21">
@@ -614,7 +614,7 @@
         <v>36546</v>
       </c>
       <c r="B22" t="n">
-        <v>4.798918249471387</v>
+        <v>4.798918249471388</v>
       </c>
     </row>
     <row r="23">
@@ -662,7 +662,7 @@
         <v>36552</v>
       </c>
       <c r="B28" t="n">
-        <v>2.18917682463635</v>
+        <v>2.189176824636349</v>
       </c>
     </row>
     <row r="29">
@@ -670,7 +670,7 @@
         <v>36553</v>
       </c>
       <c r="B29" t="n">
-        <v>0.3992773965095375</v>
+        <v>0.3992773965095374</v>
       </c>
     </row>
     <row r="30">
@@ -782,7 +782,7 @@
         <v>36567</v>
       </c>
       <c r="B43" t="n">
-        <v>1.697768414106346</v>
+        <v>1.697768414106345</v>
       </c>
     </row>
     <row r="44">
@@ -830,7 +830,7 @@
         <v>36573</v>
       </c>
       <c r="B49" t="n">
-        <v>5</v>
+        <v>4.999999999999998</v>
       </c>
     </row>
     <row r="50">
@@ -854,7 +854,7 @@
         <v>36576</v>
       </c>
       <c r="B52" t="n">
-        <v>4.838484428649334</v>
+        <v>4.838484428649335</v>
       </c>
     </row>
     <row r="53">
@@ -894,7 +894,7 @@
         <v>36581</v>
       </c>
       <c r="B57" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58">
@@ -950,7 +950,7 @@
         <v>36589</v>
       </c>
       <c r="B64" t="n">
-        <v>4.999999999999999</v>
+        <v>4.999999999999998</v>
       </c>
     </row>
     <row r="65">
@@ -974,7 +974,7 @@
         <v>36592</v>
       </c>
       <c r="B67" t="n">
-        <v>0.4166285200648882</v>
+        <v>0.4166285200648883</v>
       </c>
     </row>
     <row r="68">
@@ -1006,7 +1006,7 @@
         <v>36596</v>
       </c>
       <c r="B71" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="72">
@@ -1014,7 +1014,7 @@
         <v>36597</v>
       </c>
       <c r="B72" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="73">
@@ -1038,7 +1038,7 @@
         <v>36600</v>
       </c>
       <c r="B75" t="n">
-        <v>4.154078783986692</v>
+        <v>4.154078783986691</v>
       </c>
     </row>
     <row r="76">
@@ -1054,7 +1054,7 @@
         <v>36602</v>
       </c>
       <c r="B77" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="78">
@@ -1062,7 +1062,7 @@
         <v>36603</v>
       </c>
       <c r="B78" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="79">
@@ -1230,7 +1230,7 @@
         <v>36624</v>
       </c>
       <c r="B99" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="100">
@@ -1246,7 +1246,7 @@
         <v>36626</v>
       </c>
       <c r="B101" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="102">
@@ -1294,7 +1294,7 @@
         <v>36632</v>
       </c>
       <c r="B107" t="n">
-        <v>4.999999999999998</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="108">
@@ -1374,7 +1374,7 @@
         <v>36642</v>
       </c>
       <c r="B117" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="118">
@@ -1462,7 +1462,7 @@
         <v>36653</v>
       </c>
       <c r="B128" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="129">
@@ -1494,7 +1494,7 @@
         <v>36657</v>
       </c>
       <c r="B132" t="n">
-        <v>5</v>
+        <v>4.999999999999998</v>
       </c>
     </row>
     <row r="133">
@@ -1534,7 +1534,7 @@
         <v>36662</v>
       </c>
       <c r="B137" t="n">
-        <v>4.999999999999998</v>
+        <v>5</v>
       </c>
     </row>
     <row r="138">
@@ -1582,7 +1582,7 @@
         <v>36668</v>
       </c>
       <c r="B143" t="n">
-        <v>4.999999999999998</v>
+        <v>5</v>
       </c>
     </row>
     <row r="144">
@@ -1598,7 +1598,7 @@
         <v>36670</v>
       </c>
       <c r="B145" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="146">
@@ -1606,7 +1606,7 @@
         <v>36671</v>
       </c>
       <c r="B146" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="147">
@@ -1614,7 +1614,7 @@
         <v>36672</v>
       </c>
       <c r="B147" t="n">
-        <v>4.999999999999999</v>
+        <v>4.999999999999998</v>
       </c>
     </row>
     <row r="148">
@@ -1710,7 +1710,7 @@
         <v>36684</v>
       </c>
       <c r="B159" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="160">
@@ -1726,7 +1726,7 @@
         <v>36686</v>
       </c>
       <c r="B161" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="162">
@@ -1758,7 +1758,7 @@
         <v>36690</v>
       </c>
       <c r="B165" t="n">
-        <v>2.535179007384259</v>
+        <v>2.535179007384258</v>
       </c>
     </row>
     <row r="166">
@@ -1766,7 +1766,7 @@
         <v>36691</v>
       </c>
       <c r="B166" t="n">
-        <v>4.999999999999998</v>
+        <v>5</v>
       </c>
     </row>
     <row r="167">
@@ -1782,7 +1782,7 @@
         <v>36693</v>
       </c>
       <c r="B168" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="169">
@@ -1870,7 +1870,7 @@
         <v>36704</v>
       </c>
       <c r="B179" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="180">
@@ -1910,7 +1910,7 @@
         <v>36709</v>
       </c>
       <c r="B184" t="n">
-        <v>4.999999999999999</v>
+        <v>4.999999999999998</v>
       </c>
     </row>
     <row r="185">
@@ -1926,7 +1926,7 @@
         <v>36711</v>
       </c>
       <c r="B186" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="187">
@@ -1942,7 +1942,7 @@
         <v>36713</v>
       </c>
       <c r="B188" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="189">
@@ -1950,7 +1950,7 @@
         <v>36714</v>
       </c>
       <c r="B189" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="190">
@@ -1966,7 +1966,7 @@
         <v>36716</v>
       </c>
       <c r="B191" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="192">
@@ -1990,7 +1990,7 @@
         <v>36719</v>
       </c>
       <c r="B194" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="195">
@@ -1998,7 +1998,7 @@
         <v>36720</v>
       </c>
       <c r="B195" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="196">
@@ -2014,7 +2014,7 @@
         <v>36722</v>
       </c>
       <c r="B197" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="198">
@@ -2030,7 +2030,7 @@
         <v>36724</v>
       </c>
       <c r="B199" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="200">
@@ -2038,7 +2038,7 @@
         <v>36725</v>
       </c>
       <c r="B200" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="201">
@@ -2054,7 +2054,7 @@
         <v>36727</v>
       </c>
       <c r="B202" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="203">
@@ -2070,7 +2070,7 @@
         <v>36729</v>
       </c>
       <c r="B204" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="205">
@@ -2078,7 +2078,7 @@
         <v>36730</v>
       </c>
       <c r="B205" t="n">
-        <v>5</v>
+        <v>4.999999999999998</v>
       </c>
     </row>
     <row r="206">
@@ -2086,7 +2086,7 @@
         <v>36731</v>
       </c>
       <c r="B206" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="207">
@@ -2134,7 +2134,7 @@
         <v>36737</v>
       </c>
       <c r="B212" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="213">
@@ -2150,7 +2150,7 @@
         <v>36739</v>
       </c>
       <c r="B214" t="n">
-        <v>4.999999999999999</v>
+        <v>4.999999999999998</v>
       </c>
     </row>
     <row r="215">
@@ -2182,7 +2182,7 @@
         <v>36743</v>
       </c>
       <c r="B218" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="219">
@@ -2198,7 +2198,7 @@
         <v>36745</v>
       </c>
       <c r="B220" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="221">
@@ -2222,7 +2222,7 @@
         <v>36748</v>
       </c>
       <c r="B223" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="224">
@@ -2278,7 +2278,7 @@
         <v>36755</v>
       </c>
       <c r="B230" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="231">
@@ -2294,7 +2294,7 @@
         <v>36757</v>
       </c>
       <c r="B232" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="233">
@@ -2318,7 +2318,7 @@
         <v>36760</v>
       </c>
       <c r="B235" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="236">
@@ -2366,7 +2366,7 @@
         <v>36766</v>
       </c>
       <c r="B241" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="242">
@@ -2374,7 +2374,7 @@
         <v>36767</v>
       </c>
       <c r="B242" t="n">
-        <v>3.719346064185719</v>
+        <v>3.719346064185718</v>
       </c>
     </row>
     <row r="243">
@@ -2382,7 +2382,7 @@
         <v>36768</v>
       </c>
       <c r="B243" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="244">
@@ -2430,7 +2430,7 @@
         <v>36774</v>
       </c>
       <c r="B249" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="250">
@@ -2446,7 +2446,7 @@
         <v>36776</v>
       </c>
       <c r="B251" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="252">
@@ -2462,7 +2462,7 @@
         <v>36778</v>
       </c>
       <c r="B253" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="254">
@@ -2518,7 +2518,7 @@
         <v>36785</v>
       </c>
       <c r="B260" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="261">
@@ -2534,7 +2534,7 @@
         <v>36787</v>
       </c>
       <c r="B262" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="263">
@@ -2542,7 +2542,7 @@
         <v>36788</v>
       </c>
       <c r="B263" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="264">
@@ -2550,7 +2550,7 @@
         <v>36789</v>
       </c>
       <c r="B264" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="265">
@@ -2582,7 +2582,7 @@
         <v>36793</v>
       </c>
       <c r="B268" t="n">
-        <v>4.999999999999998</v>
+        <v>5</v>
       </c>
     </row>
     <row r="269">
@@ -2646,7 +2646,7 @@
         <v>36801</v>
       </c>
       <c r="B276" t="n">
-        <v>0.3226857506745074</v>
+        <v>0.3226857506745073</v>
       </c>
     </row>
     <row r="277">
@@ -2662,7 +2662,7 @@
         <v>36803</v>
       </c>
       <c r="B278" t="n">
-        <v>4.745134634369503</v>
+        <v>4.745134634369502</v>
       </c>
     </row>
     <row r="279">
@@ -2694,7 +2694,7 @@
         <v>36807</v>
       </c>
       <c r="B282" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="283">
@@ -2718,7 +2718,7 @@
         <v>36810</v>
       </c>
       <c r="B285" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="286">
@@ -2726,7 +2726,7 @@
         <v>36811</v>
       </c>
       <c r="B286" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="287">
@@ -2734,7 +2734,7 @@
         <v>36812</v>
       </c>
       <c r="B287" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="288">
@@ -2798,7 +2798,7 @@
         <v>36820</v>
       </c>
       <c r="B295" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="296">
@@ -2814,7 +2814,7 @@
         <v>36822</v>
       </c>
       <c r="B297" t="n">
-        <v>3.683546258631072</v>
+        <v>3.683546258631071</v>
       </c>
     </row>
     <row r="298">
@@ -2894,7 +2894,7 @@
         <v>36832</v>
       </c>
       <c r="B307" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="308">
@@ -2918,7 +2918,7 @@
         <v>36835</v>
       </c>
       <c r="B310" t="n">
-        <v>4.408428547892324</v>
+        <v>4.408428547892323</v>
       </c>
     </row>
     <row r="311">
@@ -2934,7 +2934,7 @@
         <v>36837</v>
       </c>
       <c r="B312" t="n">
-        <v>0.169440891798783</v>
+        <v>0.1694408917987829</v>
       </c>
     </row>
     <row r="313">
@@ -2966,7 +2966,7 @@
         <v>36841</v>
       </c>
       <c r="B316" t="n">
-        <v>0.4614315677556508</v>
+        <v>0.4614315677556507</v>
       </c>
     </row>
     <row r="317">
@@ -2982,7 +2982,7 @@
         <v>36843</v>
       </c>
       <c r="B318" t="n">
-        <v>3.115238810587208</v>
+        <v>3.115238810587209</v>
       </c>
     </row>
     <row r="319">
@@ -3006,7 +3006,7 @@
         <v>36846</v>
       </c>
       <c r="B321" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="322">
@@ -3014,7 +3014,7 @@
         <v>36847</v>
       </c>
       <c r="B322" t="n">
-        <v>4.535065746685913</v>
+        <v>4.535065746685911</v>
       </c>
     </row>
     <row r="323">
@@ -3030,7 +3030,7 @@
         <v>36849</v>
       </c>
       <c r="B324" t="n">
-        <v>0.6463981650075452</v>
+        <v>0.6463981650075448</v>
       </c>
     </row>
     <row r="325">
@@ -3190,7 +3190,7 @@
         <v>36869</v>
       </c>
       <c r="B344" t="n">
-        <v>0.2083672219493407</v>
+        <v>0.2083672219493406</v>
       </c>
     </row>
     <row r="345">
@@ -3198,7 +3198,7 @@
         <v>36870</v>
       </c>
       <c r="B345" t="n">
-        <v>1.667840607982242</v>
+        <v>1.667840607982241</v>
       </c>
     </row>
     <row r="346">
@@ -3294,7 +3294,7 @@
         <v>36882</v>
       </c>
       <c r="B357" t="n">
-        <v>0.05886986454951505</v>
+        <v>0.05886986454951502</v>
       </c>
     </row>
     <row r="358">
@@ -3334,7 +3334,7 @@
         <v>36887</v>
       </c>
       <c r="B362" t="n">
-        <v>1.889049547996697</v>
+        <v>1.889049547996696</v>
       </c>
     </row>
     <row r="363">
@@ -3342,7 +3342,7 @@
         <v>36888</v>
       </c>
       <c r="B363" t="n">
-        <v>2.449658431003876</v>
+        <v>2.449658431003875</v>
       </c>
     </row>
     <row r="364">

</xml_diff>

<commit_message>
EV integrated in calculating electricity cost and battery added in dynamic E cost
</commit_message>
<xml_diff>
--- a/results/end_of_day_charge_levels.xlsx
+++ b/results/end_of_day_charge_levels.xlsx
@@ -454,7 +454,7 @@
         <v>36526</v>
       </c>
       <c r="B2" t="n">
-        <v>0.6612923584120468</v>
+        <v>0.6466920752666873</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         <v>36527</v>
       </c>
       <c r="B3" t="n">
-        <v>0.059623308068666</v>
+        <v>0.1781285412312651</v>
       </c>
     </row>
     <row r="4">
@@ -470,7 +470,7 @@
         <v>36528</v>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>0.008116694847272454</v>
       </c>
     </row>
     <row r="5">
@@ -486,7 +486,7 @@
         <v>36530</v>
       </c>
       <c r="B6" t="n">
-        <v>0.06366381003880003</v>
+        <v>0.2792480393578958</v>
       </c>
     </row>
     <row r="7">
@@ -494,7 +494,7 @@
         <v>36531</v>
       </c>
       <c r="B7" t="n">
-        <v>0.3652196685519796</v>
+        <v>0.2830623685657601</v>
       </c>
     </row>
     <row r="8">
@@ -502,7 +502,7 @@
         <v>36532</v>
       </c>
       <c r="B8" t="n">
-        <v>0.04996742616246878</v>
+        <v>0.01205925836690369</v>
       </c>
     </row>
     <row r="9">
@@ -518,7 +518,7 @@
         <v>36534</v>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>0.02455928155235285</v>
       </c>
     </row>
     <row r="11">
@@ -526,7 +526,7 @@
         <v>36535</v>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>0.1786362727474556</v>
       </c>
     </row>
     <row r="12">
@@ -534,7 +534,7 @@
         <v>36536</v>
       </c>
       <c r="B12" t="n">
-        <v>0.550041762273092</v>
+        <v>0.4564972328297493</v>
       </c>
     </row>
     <row r="13">
@@ -542,7 +542,7 @@
         <v>36537</v>
       </c>
       <c r="B13" t="n">
-        <v>0.004601116908458595</v>
+        <v>0.05037649636977957</v>
       </c>
     </row>
     <row r="14">
@@ -550,7 +550,7 @@
         <v>36538</v>
       </c>
       <c r="B14" t="n">
-        <v>0.4147975016967796</v>
+        <v>1.150087190158708</v>
       </c>
     </row>
     <row r="15">
@@ -558,7 +558,7 @@
         <v>36539</v>
       </c>
       <c r="B15" t="n">
-        <v>5</v>
+        <v>2.720411860160724</v>
       </c>
     </row>
     <row r="16">
@@ -574,7 +574,7 @@
         <v>36541</v>
       </c>
       <c r="B17" t="n">
-        <v>0.7826639139786733</v>
+        <v>1.313477269125471</v>
       </c>
     </row>
     <row r="18">
@@ -582,7 +582,7 @@
         <v>36542</v>
       </c>
       <c r="B18" t="n">
-        <v>0.3017559711545987</v>
+        <v>0.6493402530349858</v>
       </c>
     </row>
     <row r="19">
@@ -590,7 +590,7 @@
         <v>36543</v>
       </c>
       <c r="B19" t="n">
-        <v>0.461896467559182</v>
+        <v>0.2787236207603832</v>
       </c>
     </row>
     <row r="20">
@@ -598,7 +598,7 @@
         <v>36544</v>
       </c>
       <c r="B20" t="n">
-        <v>2.850005230986529</v>
+        <v>3.577605081321416</v>
       </c>
     </row>
     <row r="21">
@@ -614,7 +614,7 @@
         <v>36546</v>
       </c>
       <c r="B22" t="n">
-        <v>4.798918249471388</v>
+        <v>3.335471910808629</v>
       </c>
     </row>
     <row r="23">
@@ -622,7 +622,7 @@
         <v>36547</v>
       </c>
       <c r="B23" t="n">
-        <v>0.6435353410534845</v>
+        <v>0.7558049085594679</v>
       </c>
     </row>
     <row r="24">
@@ -630,7 +630,7 @@
         <v>36548</v>
       </c>
       <c r="B24" t="n">
-        <v>1.89172556110515</v>
+        <v>2.19372556110515</v>
       </c>
     </row>
     <row r="25">
@@ -654,7 +654,7 @@
         <v>36551</v>
       </c>
       <c r="B27" t="n">
-        <v>2.052538616323845</v>
+        <v>2.125905748582776</v>
       </c>
     </row>
     <row r="28">
@@ -662,7 +662,7 @@
         <v>36552</v>
       </c>
       <c r="B28" t="n">
-        <v>2.189176824636349</v>
+        <v>2.317350895597211</v>
       </c>
     </row>
     <row r="29">
@@ -670,7 +670,7 @@
         <v>36553</v>
       </c>
       <c r="B29" t="n">
-        <v>0.3992773965095374</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -686,7 +686,7 @@
         <v>36555</v>
       </c>
       <c r="B31" t="n">
-        <v>3.588460746437567</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32">
@@ -702,7 +702,7 @@
         <v>36557</v>
       </c>
       <c r="B33" t="n">
-        <v>0.3687752225452746</v>
+        <v>0.3537752225452746</v>
       </c>
     </row>
     <row r="34">
@@ -726,7 +726,7 @@
         <v>36560</v>
       </c>
       <c r="B36" t="n">
-        <v>1.462539197539338</v>
+        <v>0.3403636535150025</v>
       </c>
     </row>
     <row r="37">
@@ -734,7 +734,7 @@
         <v>36561</v>
       </c>
       <c r="B37" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="38">
@@ -742,7 +742,7 @@
         <v>36562</v>
       </c>
       <c r="B38" t="n">
-        <v>0.06067786462378212</v>
+        <v>0.09767786462378213</v>
       </c>
     </row>
     <row r="39">
@@ -766,7 +766,7 @@
         <v>36565</v>
       </c>
       <c r="B41" t="n">
-        <v>4.290096967500113</v>
+        <v>4.826368538307462</v>
       </c>
     </row>
     <row r="42">
@@ -774,7 +774,7 @@
         <v>36566</v>
       </c>
       <c r="B42" t="n">
-        <v>1.712857906740498</v>
+        <v>1.535091466708628</v>
       </c>
     </row>
     <row r="43">
@@ -782,7 +782,7 @@
         <v>36567</v>
       </c>
       <c r="B43" t="n">
-        <v>1.697768414106345</v>
+        <v>1.247292322954824</v>
       </c>
     </row>
     <row r="44">
@@ -790,7 +790,7 @@
         <v>36568</v>
       </c>
       <c r="B44" t="n">
-        <v>2.703474551692285</v>
+        <v>3.137080194166382</v>
       </c>
     </row>
     <row r="45">
@@ -798,7 +798,7 @@
         <v>36569</v>
       </c>
       <c r="B45" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="46">
@@ -806,7 +806,7 @@
         <v>36570</v>
       </c>
       <c r="B46" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47">
@@ -814,7 +814,7 @@
         <v>36571</v>
       </c>
       <c r="B47" t="n">
-        <v>0</v>
+        <v>0.1255725322071804</v>
       </c>
     </row>
     <row r="48">
@@ -822,7 +822,7 @@
         <v>36572</v>
       </c>
       <c r="B48" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="49">
@@ -830,7 +830,7 @@
         <v>36573</v>
       </c>
       <c r="B49" t="n">
-        <v>4.999999999999998</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50">
@@ -846,7 +846,7 @@
         <v>36575</v>
       </c>
       <c r="B51" t="n">
-        <v>2.502364454120514</v>
+        <v>2.690920019497323</v>
       </c>
     </row>
     <row r="52">
@@ -854,7 +854,7 @@
         <v>36576</v>
       </c>
       <c r="B52" t="n">
-        <v>4.838484428649335</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53">
@@ -910,7 +910,7 @@
         <v>36583</v>
       </c>
       <c r="B59" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="60">
@@ -926,7 +926,7 @@
         <v>36586</v>
       </c>
       <c r="B61" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="62">
@@ -950,7 +950,7 @@
         <v>36589</v>
       </c>
       <c r="B64" t="n">
-        <v>4.999999999999998</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="65">
@@ -966,7 +966,7 @@
         <v>36591</v>
       </c>
       <c r="B66" t="n">
-        <v>3.106637722051017</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="67">
@@ -974,7 +974,7 @@
         <v>36592</v>
       </c>
       <c r="B67" t="n">
-        <v>0.4166285200648883</v>
+        <v>0.5156285200648882</v>
       </c>
     </row>
     <row r="68">
@@ -982,7 +982,7 @@
         <v>36593</v>
       </c>
       <c r="B68" t="n">
-        <v>1.45114949282424</v>
+        <v>1.624944629042829</v>
       </c>
     </row>
     <row r="69">
@@ -990,7 +990,7 @@
         <v>36594</v>
       </c>
       <c r="B69" t="n">
-        <v>2.759490757454635</v>
+        <v>4.03421817397156</v>
       </c>
     </row>
     <row r="70">
@@ -998,7 +998,7 @@
         <v>36595</v>
       </c>
       <c r="B70" t="n">
-        <v>1.867737728191094</v>
+        <v>1.837428685256278</v>
       </c>
     </row>
     <row r="71">
@@ -1006,7 +1006,7 @@
         <v>36596</v>
       </c>
       <c r="B71" t="n">
-        <v>5</v>
+        <v>3.437573465975591</v>
       </c>
     </row>
     <row r="72">
@@ -1014,7 +1014,7 @@
         <v>36597</v>
       </c>
       <c r="B72" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73">
@@ -1038,7 +1038,7 @@
         <v>36600</v>
       </c>
       <c r="B75" t="n">
-        <v>4.154078783986691</v>
+        <v>2.840218418339626</v>
       </c>
     </row>
     <row r="76">
@@ -1054,7 +1054,7 @@
         <v>36602</v>
       </c>
       <c r="B77" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="78">
@@ -1062,7 +1062,7 @@
         <v>36603</v>
       </c>
       <c r="B78" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="79">
@@ -1086,7 +1086,7 @@
         <v>36606</v>
       </c>
       <c r="B81" t="n">
-        <v>4.999999999999998</v>
+        <v>5</v>
       </c>
     </row>
     <row r="82">
@@ -1094,7 +1094,7 @@
         <v>36607</v>
       </c>
       <c r="B82" t="n">
-        <v>3.243283972901243</v>
+        <v>4.357385275081653</v>
       </c>
     </row>
     <row r="83">
@@ -1102,7 +1102,7 @@
         <v>36608</v>
       </c>
       <c r="B83" t="n">
-        <v>3.326071396160306</v>
+        <v>2.478425057904969</v>
       </c>
     </row>
     <row r="84">
@@ -1126,7 +1126,7 @@
         <v>36611</v>
       </c>
       <c r="B86" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="87">
@@ -1134,7 +1134,7 @@
         <v>36612</v>
       </c>
       <c r="B87" t="n">
-        <v>2.445417018975182</v>
+        <v>3.065234955861487</v>
       </c>
     </row>
     <row r="88">
@@ -1182,7 +1182,7 @@
         <v>36618</v>
       </c>
       <c r="B93" t="n">
-        <v>4.480980874603226</v>
+        <v>4.134562471626321</v>
       </c>
     </row>
     <row r="94">
@@ -1190,7 +1190,7 @@
         <v>36619</v>
       </c>
       <c r="B94" t="n">
-        <v>3.580172807626497</v>
+        <v>4.932602540833704</v>
       </c>
     </row>
     <row r="95">
@@ -1198,7 +1198,7 @@
         <v>36620</v>
       </c>
       <c r="B95" t="n">
-        <v>2.37417902841104</v>
+        <v>2.717070706888844</v>
       </c>
     </row>
     <row r="96">
@@ -1222,7 +1222,7 @@
         <v>36623</v>
       </c>
       <c r="B98" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="99">
@@ -1238,7 +1238,7 @@
         <v>36625</v>
       </c>
       <c r="B100" t="n">
-        <v>3.98751372195797</v>
+        <v>4.443183656811081</v>
       </c>
     </row>
     <row r="101">
@@ -1254,7 +1254,7 @@
         <v>36627</v>
       </c>
       <c r="B102" t="n">
-        <v>1.973395096959228</v>
+        <v>1.748395096959228</v>
       </c>
     </row>
     <row r="103">
@@ -1262,7 +1262,7 @@
         <v>36628</v>
       </c>
       <c r="B103" t="n">
-        <v>3.854291003672147</v>
+        <v>3.595087166888811</v>
       </c>
     </row>
     <row r="104">
@@ -1294,7 +1294,7 @@
         <v>36632</v>
       </c>
       <c r="B107" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="108">
@@ -1326,7 +1326,7 @@
         <v>36636</v>
       </c>
       <c r="B111" t="n">
-        <v>5</v>
+        <v>4.999999999999997</v>
       </c>
     </row>
     <row r="112">
@@ -1374,7 +1374,7 @@
         <v>36642</v>
       </c>
       <c r="B117" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="118">
@@ -1406,7 +1406,7 @@
         <v>36646</v>
       </c>
       <c r="B121" t="n">
-        <v>4.510137868980221</v>
+        <v>4.496967566312717</v>
       </c>
     </row>
     <row r="122">
@@ -1414,7 +1414,7 @@
         <v>36647</v>
       </c>
       <c r="B122" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="123">
@@ -1470,7 +1470,7 @@
         <v>36654</v>
       </c>
       <c r="B129" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="130">
@@ -1486,7 +1486,7 @@
         <v>36656</v>
       </c>
       <c r="B131" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="132">
@@ -1494,7 +1494,7 @@
         <v>36657</v>
       </c>
       <c r="B132" t="n">
-        <v>4.999999999999998</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="133">
@@ -1566,7 +1566,7 @@
         <v>36666</v>
       </c>
       <c r="B141" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="142">
@@ -1582,7 +1582,7 @@
         <v>36668</v>
       </c>
       <c r="B143" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="144">
@@ -1670,7 +1670,7 @@
         <v>36679</v>
       </c>
       <c r="B154" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="155">
@@ -1694,7 +1694,7 @@
         <v>36682</v>
       </c>
       <c r="B157" t="n">
-        <v>4.759199051761575</v>
+        <v>5</v>
       </c>
     </row>
     <row r="158">
@@ -1710,7 +1710,7 @@
         <v>36684</v>
       </c>
       <c r="B159" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="160">
@@ -1726,7 +1726,7 @@
         <v>36686</v>
       </c>
       <c r="B161" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="162">
@@ -1734,7 +1734,7 @@
         <v>36687</v>
       </c>
       <c r="B162" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="163">
@@ -1742,7 +1742,7 @@
         <v>36688</v>
       </c>
       <c r="B163" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="164">
@@ -1750,7 +1750,7 @@
         <v>36689</v>
       </c>
       <c r="B164" t="n">
-        <v>1.964084540168082</v>
+        <v>2.161084540168082</v>
       </c>
     </row>
     <row r="165">
@@ -1758,7 +1758,7 @@
         <v>36690</v>
       </c>
       <c r="B165" t="n">
-        <v>2.535179007384258</v>
+        <v>2.552179007384258</v>
       </c>
     </row>
     <row r="166">
@@ -1782,7 +1782,7 @@
         <v>36693</v>
       </c>
       <c r="B168" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="169">
@@ -1798,7 +1798,7 @@
         <v>36695</v>
       </c>
       <c r="B170" t="n">
-        <v>3.043266336666568</v>
+        <v>2.813322979402961</v>
       </c>
     </row>
     <row r="171">
@@ -1814,7 +1814,7 @@
         <v>36697</v>
       </c>
       <c r="B172" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="173">
@@ -1822,7 +1822,7 @@
         <v>36698</v>
       </c>
       <c r="B173" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="174">
@@ -1838,7 +1838,7 @@
         <v>36700</v>
       </c>
       <c r="B175" t="n">
-        <v>1.942000742333645</v>
+        <v>1.675084540168082</v>
       </c>
     </row>
     <row r="176">
@@ -1846,7 +1846,7 @@
         <v>36701</v>
       </c>
       <c r="B176" t="n">
-        <v>3.950490898271326</v>
+        <v>2.556748441191167</v>
       </c>
     </row>
     <row r="177">
@@ -1878,7 +1878,7 @@
         <v>36705</v>
       </c>
       <c r="B180" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="181">
@@ -1886,7 +1886,7 @@
         <v>36706</v>
       </c>
       <c r="B181" t="n">
-        <v>4.145487026351776</v>
+        <v>3.639723738357389</v>
       </c>
     </row>
     <row r="182">
@@ -1894,7 +1894,7 @@
         <v>36707</v>
       </c>
       <c r="B182" t="n">
-        <v>0.2922529296163545</v>
+        <v>0.1980580145890633</v>
       </c>
     </row>
     <row r="183">
@@ -1902,7 +1902,7 @@
         <v>36708</v>
       </c>
       <c r="B183" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="184">
@@ -1910,7 +1910,7 @@
         <v>36709</v>
       </c>
       <c r="B184" t="n">
-        <v>4.999999999999998</v>
+        <v>5</v>
       </c>
     </row>
     <row r="185">
@@ -1918,7 +1918,7 @@
         <v>36710</v>
       </c>
       <c r="B185" t="n">
-        <v>5</v>
+        <v>4.999999999999998</v>
       </c>
     </row>
     <row r="186">
@@ -1926,7 +1926,7 @@
         <v>36711</v>
       </c>
       <c r="B186" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="187">
@@ -1934,7 +1934,7 @@
         <v>36712</v>
       </c>
       <c r="B187" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="188">
@@ -1974,7 +1974,7 @@
         <v>36717</v>
       </c>
       <c r="B192" t="n">
-        <v>1.237207265218224</v>
+        <v>1.085600489032491</v>
       </c>
     </row>
     <row r="193">
@@ -1990,7 +1990,7 @@
         <v>36719</v>
       </c>
       <c r="B194" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="195">
@@ -1998,7 +1998,7 @@
         <v>36720</v>
       </c>
       <c r="B195" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="196">
@@ -2006,7 +2006,7 @@
         <v>36721</v>
       </c>
       <c r="B196" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="197">
@@ -2038,7 +2038,7 @@
         <v>36725</v>
       </c>
       <c r="B200" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="201">
@@ -2054,7 +2054,7 @@
         <v>36727</v>
       </c>
       <c r="B202" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="203">
@@ -2078,7 +2078,7 @@
         <v>36730</v>
       </c>
       <c r="B205" t="n">
-        <v>4.999999999999998</v>
+        <v>5</v>
       </c>
     </row>
     <row r="206">
@@ -2086,7 +2086,7 @@
         <v>36731</v>
       </c>
       <c r="B206" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="207">
@@ -2110,7 +2110,7 @@
         <v>36734</v>
       </c>
       <c r="B209" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="210">
@@ -2134,7 +2134,7 @@
         <v>36737</v>
       </c>
       <c r="B212" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="213">
@@ -2150,7 +2150,7 @@
         <v>36739</v>
       </c>
       <c r="B214" t="n">
-        <v>4.999999999999998</v>
+        <v>5</v>
       </c>
     </row>
     <row r="215">
@@ -2166,7 +2166,7 @@
         <v>36741</v>
       </c>
       <c r="B216" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="217">
@@ -2182,7 +2182,7 @@
         <v>36743</v>
       </c>
       <c r="B218" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="219">
@@ -2198,7 +2198,7 @@
         <v>36745</v>
       </c>
       <c r="B220" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="221">
@@ -2206,7 +2206,7 @@
         <v>36746</v>
       </c>
       <c r="B221" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="222">
@@ -2222,7 +2222,7 @@
         <v>36748</v>
       </c>
       <c r="B223" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="224">
@@ -2230,7 +2230,7 @@
         <v>36749</v>
       </c>
       <c r="B224" t="n">
-        <v>5</v>
+        <v>4.999999999999998</v>
       </c>
     </row>
     <row r="225">
@@ -2238,7 +2238,7 @@
         <v>36750</v>
       </c>
       <c r="B225" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="226">
@@ -2246,7 +2246,7 @@
         <v>36751</v>
       </c>
       <c r="B226" t="n">
-        <v>5</v>
+        <v>4.976698289799462</v>
       </c>
     </row>
     <row r="227">
@@ -2254,7 +2254,7 @@
         <v>36752</v>
       </c>
       <c r="B227" t="n">
-        <v>3.107732996707481</v>
+        <v>4.830120437256947</v>
       </c>
     </row>
     <row r="228">
@@ -2262,7 +2262,7 @@
         <v>36753</v>
       </c>
       <c r="B228" t="n">
-        <v>3.177908462768261</v>
+        <v>4.408510935096554</v>
       </c>
     </row>
     <row r="229">
@@ -2270,7 +2270,7 @@
         <v>36754</v>
       </c>
       <c r="B229" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="230">
@@ -2286,7 +2286,7 @@
         <v>36756</v>
       </c>
       <c r="B231" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="232">
@@ -2302,7 +2302,7 @@
         <v>36758</v>
       </c>
       <c r="B233" t="n">
-        <v>0.164111977500803</v>
+        <v>0.1232850097561245</v>
       </c>
     </row>
     <row r="234">
@@ -2318,7 +2318,7 @@
         <v>36760</v>
       </c>
       <c r="B235" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="236">
@@ -2334,7 +2334,7 @@
         <v>36762</v>
       </c>
       <c r="B237" t="n">
-        <v>5</v>
+        <v>4.999999999999998</v>
       </c>
     </row>
     <row r="238">
@@ -2358,7 +2358,7 @@
         <v>36765</v>
       </c>
       <c r="B240" t="n">
-        <v>4.410075120886997</v>
+        <v>5</v>
       </c>
     </row>
     <row r="241">
@@ -2374,7 +2374,7 @@
         <v>36767</v>
       </c>
       <c r="B242" t="n">
-        <v>3.719346064185718</v>
+        <v>4.562036250703845</v>
       </c>
     </row>
     <row r="243">
@@ -2382,7 +2382,7 @@
         <v>36768</v>
       </c>
       <c r="B243" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="244">
@@ -2390,7 +2390,7 @@
         <v>36769</v>
       </c>
       <c r="B244" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="245">
@@ -2414,7 +2414,7 @@
         <v>36772</v>
       </c>
       <c r="B247" t="n">
-        <v>2.419986095587267</v>
+        <v>2.617719592027496</v>
       </c>
     </row>
     <row r="248">
@@ -2430,7 +2430,7 @@
         <v>36774</v>
       </c>
       <c r="B249" t="n">
-        <v>4.999999999999999</v>
+        <v>4.999999999999998</v>
       </c>
     </row>
     <row r="250">
@@ -2438,7 +2438,7 @@
         <v>36775</v>
       </c>
       <c r="B250" t="n">
-        <v>2.803669442014556</v>
+        <v>2.724626906632113</v>
       </c>
     </row>
     <row r="251">
@@ -2446,7 +2446,7 @@
         <v>36776</v>
       </c>
       <c r="B251" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="252">
@@ -2462,7 +2462,7 @@
         <v>36778</v>
       </c>
       <c r="B253" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="254">
@@ -2486,7 +2486,7 @@
         <v>36781</v>
       </c>
       <c r="B256" t="n">
-        <v>2.867882476700038</v>
+        <v>2.882687548651024</v>
       </c>
     </row>
     <row r="257">
@@ -2494,7 +2494,7 @@
         <v>36782</v>
       </c>
       <c r="B257" t="n">
-        <v>4.136052217496371</v>
+        <v>3.750026597360309</v>
       </c>
     </row>
     <row r="258">
@@ -2502,7 +2502,7 @@
         <v>36783</v>
       </c>
       <c r="B258" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="259">
@@ -2510,7 +2510,7 @@
         <v>36784</v>
       </c>
       <c r="B259" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="260">
@@ -2518,7 +2518,7 @@
         <v>36785</v>
       </c>
       <c r="B260" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="261">
@@ -2550,7 +2550,7 @@
         <v>36789</v>
       </c>
       <c r="B264" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="265">
@@ -2558,7 +2558,7 @@
         <v>36790</v>
       </c>
       <c r="B265" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="266">
@@ -2566,7 +2566,7 @@
         <v>36791</v>
       </c>
       <c r="B266" t="n">
-        <v>4.596364078714711</v>
+        <v>4.094683208233877</v>
       </c>
     </row>
     <row r="267">
@@ -2590,7 +2590,7 @@
         <v>36794</v>
       </c>
       <c r="B269" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="270">
@@ -2614,7 +2614,7 @@
         <v>36797</v>
       </c>
       <c r="B272" t="n">
-        <v>2.300314254538993</v>
+        <v>2.230754701885467</v>
       </c>
     </row>
     <row r="273">
@@ -2622,7 +2622,7 @@
         <v>36798</v>
       </c>
       <c r="B273" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="274">
@@ -2630,7 +2630,7 @@
         <v>36799</v>
       </c>
       <c r="B274" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="275">
@@ -2638,7 +2638,7 @@
         <v>36800</v>
       </c>
       <c r="B275" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="276">
@@ -2646,7 +2646,7 @@
         <v>36801</v>
       </c>
       <c r="B276" t="n">
-        <v>0.3226857506745073</v>
+        <v>0.6844996766540014</v>
       </c>
     </row>
     <row r="277">
@@ -2662,7 +2662,7 @@
         <v>36803</v>
       </c>
       <c r="B278" t="n">
-        <v>4.745134634369502</v>
+        <v>4.624661574827089</v>
       </c>
     </row>
     <row r="279">
@@ -2670,7 +2670,7 @@
         <v>36804</v>
       </c>
       <c r="B279" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="280">
@@ -2678,7 +2678,7 @@
         <v>36805</v>
       </c>
       <c r="B280" t="n">
-        <v>5</v>
+        <v>4.999999999999997</v>
       </c>
     </row>
     <row r="281">
@@ -2686,7 +2686,7 @@
         <v>36806</v>
       </c>
       <c r="B281" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="282">
@@ -2694,7 +2694,7 @@
         <v>36807</v>
       </c>
       <c r="B282" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="283">
@@ -2710,7 +2710,7 @@
         <v>36809</v>
       </c>
       <c r="B284" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="285">
@@ -2734,7 +2734,7 @@
         <v>36812</v>
       </c>
       <c r="B287" t="n">
-        <v>4.999999999999999</v>
+        <v>4.999999999999998</v>
       </c>
     </row>
     <row r="288">
@@ -2742,7 +2742,7 @@
         <v>36813</v>
       </c>
       <c r="B288" t="n">
-        <v>5</v>
+        <v>4.999999999999998</v>
       </c>
     </row>
     <row r="289">
@@ -2750,7 +2750,7 @@
         <v>36814</v>
       </c>
       <c r="B289" t="n">
-        <v>5</v>
+        <v>4.999999999999997</v>
       </c>
     </row>
     <row r="290">
@@ -2758,7 +2758,7 @@
         <v>36815</v>
       </c>
       <c r="B290" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="291">
@@ -2766,7 +2766,7 @@
         <v>36816</v>
       </c>
       <c r="B291" t="n">
-        <v>5</v>
+        <v>4.999999999999999</v>
       </c>
     </row>
     <row r="292">
@@ -2774,7 +2774,7 @@
         <v>36817</v>
       </c>
       <c r="B292" t="n">
-        <v>4.305842792303898</v>
+        <v>3.720270564180553</v>
       </c>
     </row>
     <row r="293">
@@ -2782,7 +2782,7 @@
         <v>36818</v>
       </c>
       <c r="B293" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="294">
@@ -2806,7 +2806,7 @@
         <v>36821</v>
       </c>
       <c r="B296" t="n">
-        <v>3.680321610906526</v>
+        <v>4.781491256184114</v>
       </c>
     </row>
     <row r="297">
@@ -2814,7 +2814,7 @@
         <v>36822</v>
       </c>
       <c r="B297" t="n">
-        <v>3.683546258631071</v>
+        <v>3.890777344708895</v>
       </c>
     </row>
     <row r="298">
@@ -2822,7 +2822,7 @@
         <v>36823</v>
       </c>
       <c r="B298" t="n">
-        <v>0.7132873572634397</v>
+        <v>0.3905295135920384</v>
       </c>
     </row>
     <row r="299">
@@ -2838,7 +2838,7 @@
         <v>36825</v>
       </c>
       <c r="B300" t="n">
-        <v>0.1192856732773341</v>
+        <v>0.1152856732773341</v>
       </c>
     </row>
     <row r="301">
@@ -2846,7 +2846,7 @@
         <v>36826</v>
       </c>
       <c r="B301" t="n">
-        <v>3.591054272360362</v>
+        <v>3.781466779390591</v>
       </c>
     </row>
     <row r="302">
@@ -2854,7 +2854,7 @@
         <v>36827</v>
       </c>
       <c r="B302" t="n">
-        <v>5</v>
+        <v>3.987975997351776</v>
       </c>
     </row>
     <row r="303">
@@ -2878,7 +2878,7 @@
         <v>36830</v>
       </c>
       <c r="B305" t="n">
-        <v>2.454299652530172</v>
+        <v>3.00023061163535</v>
       </c>
     </row>
     <row r="306">
@@ -2894,7 +2894,7 @@
         <v>36832</v>
       </c>
       <c r="B307" t="n">
-        <v>4.999999999999999</v>
+        <v>5</v>
       </c>
     </row>
     <row r="308">
@@ -2902,7 +2902,7 @@
         <v>36833</v>
       </c>
       <c r="B308" t="n">
-        <v>5</v>
+        <v>4.930541655522323</v>
       </c>
     </row>
     <row r="309">
@@ -2910,7 +2910,7 @@
         <v>36834</v>
       </c>
       <c r="B309" t="n">
-        <v>5</v>
+        <v>4.829458304315041</v>
       </c>
     </row>
     <row r="310">
@@ -2918,7 +2918,7 @@
         <v>36835</v>
       </c>
       <c r="B310" t="n">
-        <v>4.408428547892323</v>
+        <v>5</v>
       </c>
     </row>
     <row r="311">
@@ -2926,7 +2926,7 @@
         <v>36836</v>
       </c>
       <c r="B311" t="n">
-        <v>2.917651420098768</v>
+        <v>4.109537616051316</v>
       </c>
     </row>
     <row r="312">
@@ -2934,7 +2934,7 @@
         <v>36837</v>
       </c>
       <c r="B312" t="n">
-        <v>0.1694408917987829</v>
+        <v>0.1935457240585318</v>
       </c>
     </row>
     <row r="313">
@@ -2950,7 +2950,7 @@
         <v>36839</v>
       </c>
       <c r="B314" t="n">
-        <v>3.254444452712067</v>
+        <v>3.150168325100286</v>
       </c>
     </row>
     <row r="315">
@@ -2958,7 +2958,7 @@
         <v>36840</v>
       </c>
       <c r="B315" t="n">
-        <v>0.07596338590854232</v>
+        <v>0.02296338590854233</v>
       </c>
     </row>
     <row r="316">
@@ -2966,7 +2966,7 @@
         <v>36841</v>
       </c>
       <c r="B316" t="n">
-        <v>0.4614315677556507</v>
+        <v>1.231585024249513</v>
       </c>
     </row>
     <row r="317">
@@ -2982,7 +2982,7 @@
         <v>36843</v>
       </c>
       <c r="B318" t="n">
-        <v>3.115238810587209</v>
+        <v>2.74259459609352</v>
       </c>
     </row>
     <row r="319">
@@ -2998,7 +2998,7 @@
         <v>36845</v>
       </c>
       <c r="B320" t="n">
-        <v>5</v>
+        <v>4.557653946089296</v>
       </c>
     </row>
     <row r="321">
@@ -3014,7 +3014,7 @@
         <v>36847</v>
       </c>
       <c r="B322" t="n">
-        <v>4.535065746685911</v>
+        <v>4.641885678864514</v>
       </c>
     </row>
     <row r="323">
@@ -3022,7 +3022,7 @@
         <v>36848</v>
       </c>
       <c r="B323" t="n">
-        <v>5</v>
+        <v>4.623542858366296</v>
       </c>
     </row>
     <row r="324">
@@ -3030,7 +3030,7 @@
         <v>36849</v>
       </c>
       <c r="B324" t="n">
-        <v>0.6463981650075448</v>
+        <v>0.9045241003871236</v>
       </c>
     </row>
     <row r="325">
@@ -3046,7 +3046,7 @@
         <v>36851</v>
       </c>
       <c r="B326" t="n">
-        <v>0.5943630520730818</v>
+        <v>0.5612092702770545</v>
       </c>
     </row>
     <row r="327">
@@ -3054,7 +3054,7 @@
         <v>36852</v>
       </c>
       <c r="B327" t="n">
-        <v>5</v>
+        <v>3.707079793836671</v>
       </c>
     </row>
     <row r="328">
@@ -3062,7 +3062,7 @@
         <v>36853</v>
       </c>
       <c r="B328" t="n">
-        <v>3.744167604732198</v>
+        <v>4.402248636681061</v>
       </c>
     </row>
     <row r="329">
@@ -3094,7 +3094,7 @@
         <v>36857</v>
       </c>
       <c r="B332" t="n">
-        <v>0.1955607768787193</v>
+        <v>0.2408759839757466</v>
       </c>
     </row>
     <row r="333">
@@ -3118,7 +3118,7 @@
         <v>36860</v>
       </c>
       <c r="B335" t="n">
-        <v>0.6198220611193987</v>
+        <v>0.562679266604711</v>
       </c>
     </row>
     <row r="336">
@@ -3126,7 +3126,7 @@
         <v>36861</v>
       </c>
       <c r="B336" t="n">
-        <v>0.5056632075671252</v>
+        <v>0.5186632075671253</v>
       </c>
     </row>
     <row r="337">
@@ -3142,7 +3142,7 @@
         <v>36863</v>
       </c>
       <c r="B338" t="n">
-        <v>0.3600015234434402</v>
+        <v>0.4414928712939434</v>
       </c>
     </row>
     <row r="339">
@@ -3150,7 +3150,7 @@
         <v>36864</v>
       </c>
       <c r="B339" t="n">
-        <v>1.68162993462372</v>
+        <v>2.152401760756345</v>
       </c>
     </row>
     <row r="340">
@@ -3158,7 +3158,7 @@
         <v>36865</v>
       </c>
       <c r="B340" t="n">
-        <v>0.392076332707383</v>
+        <v>0.1894673825025871</v>
       </c>
     </row>
     <row r="341">
@@ -3190,7 +3190,7 @@
         <v>36869</v>
       </c>
       <c r="B344" t="n">
-        <v>0.2083672219493406</v>
+        <v>0</v>
       </c>
     </row>
     <row r="345">
@@ -3198,7 +3198,7 @@
         <v>36870</v>
       </c>
       <c r="B345" t="n">
-        <v>1.667840607982241</v>
+        <v>3.096727410907626</v>
       </c>
     </row>
     <row r="346">
@@ -3206,7 +3206,7 @@
         <v>36871</v>
       </c>
       <c r="B346" t="n">
-        <v>1.116643748855297</v>
+        <v>2.680575245408471</v>
       </c>
     </row>
     <row r="347">
@@ -3214,7 +3214,7 @@
         <v>36872</v>
       </c>
       <c r="B347" t="n">
-        <v>0.4260098091421166</v>
+        <v>0.3153147057440679</v>
       </c>
     </row>
     <row r="348">
@@ -3222,7 +3222,7 @@
         <v>36873</v>
       </c>
       <c r="B348" t="n">
-        <v>3.385426715545751</v>
+        <v>1.928403851722112</v>
       </c>
     </row>
     <row r="349">
@@ -3230,7 +3230,7 @@
         <v>36874</v>
       </c>
       <c r="B349" t="n">
-        <v>0.001317988031008764</v>
+        <v>0.03592429281611044</v>
       </c>
     </row>
     <row r="350">
@@ -3238,7 +3238,7 @@
         <v>36875</v>
       </c>
       <c r="B350" t="n">
-        <v>0.2894244325588191</v>
+        <v>0</v>
       </c>
     </row>
     <row r="351">
@@ -3246,7 +3246,7 @@
         <v>36876</v>
       </c>
       <c r="B351" t="n">
-        <v>0.3601049649019782</v>
+        <v>0.1606947225355558</v>
       </c>
     </row>
     <row r="352">
@@ -3254,7 +3254,7 @@
         <v>36877</v>
       </c>
       <c r="B352" t="n">
-        <v>0.1250022082417895</v>
+        <v>0.450880377995852</v>
       </c>
     </row>
     <row r="353">
@@ -3262,7 +3262,7 @@
         <v>36878</v>
       </c>
       <c r="B353" t="n">
-        <v>1.509385703163791</v>
+        <v>2.86745086343957</v>
       </c>
     </row>
     <row r="354">
@@ -3294,7 +3294,7 @@
         <v>36882</v>
       </c>
       <c r="B357" t="n">
-        <v>0.05886986454951502</v>
+        <v>0.2349863924702057</v>
       </c>
     </row>
     <row r="358">
@@ -3310,7 +3310,7 @@
         <v>36884</v>
       </c>
       <c r="B359" t="n">
-        <v>1.449449116031491</v>
+        <v>1.482432143690734</v>
       </c>
     </row>
     <row r="360">
@@ -3318,7 +3318,7 @@
         <v>36885</v>
       </c>
       <c r="B360" t="n">
-        <v>1.423522999159199</v>
+        <v>1.754996312875319</v>
       </c>
     </row>
     <row r="361">
@@ -3326,7 +3326,7 @@
         <v>36886</v>
       </c>
       <c r="B361" t="n">
-        <v>2.933660475382339</v>
+        <v>2.902617763707542</v>
       </c>
     </row>
     <row r="362">
@@ -3334,7 +3334,7 @@
         <v>36887</v>
       </c>
       <c r="B362" t="n">
-        <v>1.889049547996696</v>
+        <v>1.117834436890867</v>
       </c>
     </row>
     <row r="363">
@@ -3342,7 +3342,7 @@
         <v>36888</v>
       </c>
       <c r="B363" t="n">
-        <v>2.449658431003875</v>
+        <v>3.180780615500789</v>
       </c>
     </row>
     <row r="364">
@@ -3358,7 +3358,7 @@
         <v>36890</v>
       </c>
       <c r="B365" t="n">
-        <v>0.05353113140634157</v>
+        <v>0.002638625277041312</v>
       </c>
     </row>
     <row r="366">

</xml_diff>

<commit_message>
Final financial evaluation (hopefully)
</commit_message>
<xml_diff>
--- a/results/end_of_day_charge_levels.xlsx
+++ b/results/end_of_day_charge_levels.xlsx
@@ -454,7 +454,7 @@
         <v>36526</v>
       </c>
       <c r="B2" t="n">
-        <v>1.753615645817214</v>
+        <v>1.75323082413364</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         <v>36527</v>
       </c>
       <c r="B3" t="n">
-        <v>0.5938842625794604</v>
+        <v>0.593878134705203</v>
       </c>
     </row>
     <row r="4">
@@ -470,7 +470,7 @@
         <v>36528</v>
       </c>
       <c r="B4" t="n">
-        <v>0.08971896248424925</v>
+        <v>0.08968573812503104</v>
       </c>
     </row>
     <row r="5">
@@ -486,7 +486,7 @@
         <v>36530</v>
       </c>
       <c r="B6" t="n">
-        <v>0.6979638715554557</v>
+        <v>0.697984212789899</v>
       </c>
     </row>
     <row r="7">
@@ -494,7 +494,7 @@
         <v>36531</v>
       </c>
       <c r="B7" t="n">
-        <v>1.467659115967847</v>
+        <v>1.46766230453241</v>
       </c>
     </row>
     <row r="8">
@@ -502,7 +502,7 @@
         <v>36532</v>
       </c>
       <c r="B8" t="n">
-        <v>0.1529104582623473</v>
+        <v>0.1529174153094237</v>
       </c>
     </row>
     <row r="9">
@@ -518,7 +518,7 @@
         <v>36534</v>
       </c>
       <c r="B10" t="n">
-        <v>0.1315652310223139</v>
+        <v>0.13157929771114</v>
       </c>
     </row>
     <row r="11">
@@ -526,7 +526,7 @@
         <v>36535</v>
       </c>
       <c r="B11" t="n">
-        <v>0.6509388395566055</v>
+        <v>0.6509370398033711</v>
       </c>
     </row>
     <row r="12">
@@ -534,7 +534,7 @@
         <v>36536</v>
       </c>
       <c r="B12" t="n">
-        <v>1.461255188837675</v>
+        <v>1.461328053379982</v>
       </c>
     </row>
     <row r="13">
@@ -542,7 +542,7 @@
         <v>36537</v>
       </c>
       <c r="B13" t="n">
-        <v>0.4288573366235478</v>
+        <v>0.4288601029876928</v>
       </c>
     </row>
     <row r="14">
@@ -550,7 +550,7 @@
         <v>36538</v>
       </c>
       <c r="B14" t="n">
-        <v>2.884960243775851</v>
+        <v>2.885157388118126</v>
       </c>
     </row>
     <row r="15">
@@ -558,7 +558,7 @@
         <v>36539</v>
       </c>
       <c r="B15" t="n">
-        <v>6.499999999999998</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="16">
@@ -574,7 +574,7 @@
         <v>36541</v>
       </c>
       <c r="B17" t="n">
-        <v>3.180824786953745</v>
+        <v>3.180972128531454</v>
       </c>
     </row>
     <row r="18">
@@ -582,7 +582,7 @@
         <v>36542</v>
       </c>
       <c r="B18" t="n">
-        <v>1.718840042950984</v>
+        <v>1.719203426536505</v>
       </c>
     </row>
     <row r="19">
@@ -590,7 +590,7 @@
         <v>36543</v>
       </c>
       <c r="B19" t="n">
-        <v>1.019325843492061</v>
+        <v>1.019312221171229</v>
       </c>
     </row>
     <row r="20">
@@ -622,7 +622,7 @@
         <v>36547</v>
       </c>
       <c r="B23" t="n">
-        <v>2.12549077014323</v>
+        <v>2.125499243304335</v>
       </c>
     </row>
     <row r="24">
@@ -630,7 +630,7 @@
         <v>36548</v>
       </c>
       <c r="B24" t="n">
-        <v>4.981274644458361</v>
+        <v>4.98132897624707</v>
       </c>
     </row>
     <row r="25">
@@ -654,7 +654,7 @@
         <v>36551</v>
       </c>
       <c r="B27" t="n">
-        <v>5.58545707656323</v>
+        <v>5.585462082187729</v>
       </c>
     </row>
     <row r="28">
@@ -670,7 +670,7 @@
         <v>36553</v>
       </c>
       <c r="B29" t="n">
-        <v>0.3622973446055163</v>
+        <v>0.3623348664826305</v>
       </c>
     </row>
     <row r="30">
@@ -686,7 +686,7 @@
         <v>36555</v>
       </c>
       <c r="B31" t="n">
-        <v>6.499999999999999</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="32">
@@ -702,7 +702,7 @@
         <v>36557</v>
       </c>
       <c r="B33" t="n">
-        <v>1.011324717773969</v>
+        <v>1.011616799548485</v>
       </c>
     </row>
     <row r="34">
@@ -726,7 +726,7 @@
         <v>36560</v>
       </c>
       <c r="B36" t="n">
-        <v>2.118445757397316</v>
+        <v>2.117756230182099</v>
       </c>
     </row>
     <row r="37">
@@ -742,7 +742,7 @@
         <v>36562</v>
       </c>
       <c r="B38" t="n">
-        <v>0.3824128319014202</v>
+        <v>0.3824165731505474</v>
       </c>
     </row>
     <row r="39">
@@ -774,7 +774,7 @@
         <v>36566</v>
       </c>
       <c r="B42" t="n">
-        <v>4.277220215788186</v>
+        <v>4.279384958374867</v>
       </c>
     </row>
     <row r="43">
@@ -782,7 +782,7 @@
         <v>36567</v>
       </c>
       <c r="B43" t="n">
-        <v>3.988655836925938</v>
+        <v>3.989456209561919</v>
       </c>
     </row>
     <row r="44">
@@ -806,7 +806,7 @@
         <v>36570</v>
       </c>
       <c r="B46" t="n">
-        <v>6.499999999999999</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="47">
@@ -814,7 +814,7 @@
         <v>36571</v>
       </c>
       <c r="B47" t="n">
-        <v>0.3941193393099126</v>
+        <v>0.3941827851409692</v>
       </c>
     </row>
     <row r="48">
@@ -838,7 +838,7 @@
         <v>36574</v>
       </c>
       <c r="B50" t="n">
-        <v>6.5</v>
+        <v>6.499999999999999</v>
       </c>
     </row>
     <row r="51">
@@ -846,7 +846,7 @@
         <v>36575</v>
       </c>
       <c r="B51" t="n">
-        <v>6.499999999999999</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="52">
@@ -854,7 +854,7 @@
         <v>36576</v>
       </c>
       <c r="B52" t="n">
-        <v>6.5</v>
+        <v>6.499999999999999</v>
       </c>
     </row>
     <row r="53">
@@ -958,7 +958,7 @@
         <v>36590</v>
       </c>
       <c r="B65" t="n">
-        <v>6.5</v>
+        <v>6.499999999999998</v>
       </c>
     </row>
     <row r="66">
@@ -974,7 +974,7 @@
         <v>36592</v>
       </c>
       <c r="B67" t="n">
-        <v>1.480953089049003</v>
+        <v>1.480927694737103</v>
       </c>
     </row>
     <row r="68">
@@ -982,7 +982,7 @@
         <v>36593</v>
       </c>
       <c r="B68" t="n">
-        <v>4.416397235855274</v>
+        <v>4.416900120215068</v>
       </c>
     </row>
     <row r="69">
@@ -990,7 +990,7 @@
         <v>36594</v>
       </c>
       <c r="B69" t="n">
-        <v>6.499999999999999</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="70">
@@ -998,7 +998,7 @@
         <v>36595</v>
       </c>
       <c r="B70" t="n">
-        <v>4.878304752335495</v>
+        <v>4.878275420122094</v>
       </c>
     </row>
     <row r="71">
@@ -1006,7 +1006,7 @@
         <v>36596</v>
       </c>
       <c r="B71" t="n">
-        <v>6.499999999999998</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="72">
@@ -1046,7 +1046,7 @@
         <v>36601</v>
       </c>
       <c r="B76" t="n">
-        <v>0.004237689235349201</v>
+        <v>0.004237524799288225</v>
       </c>
     </row>
     <row r="77">
@@ -1086,7 +1086,7 @@
         <v>36606</v>
       </c>
       <c r="B81" t="n">
-        <v>6.499999999999998</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="82">
@@ -1094,7 +1094,7 @@
         <v>36607</v>
       </c>
       <c r="B82" t="n">
-        <v>6.5</v>
+        <v>6.499999999999999</v>
       </c>
     </row>
     <row r="83">
@@ -1102,7 +1102,7 @@
         <v>36608</v>
       </c>
       <c r="B83" t="n">
-        <v>6.499999999999998</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="84">
@@ -1150,7 +1150,7 @@
         <v>36614</v>
       </c>
       <c r="B89" t="n">
-        <v>6.5</v>
+        <v>6.499999999999999</v>
       </c>
     </row>
     <row r="90">
@@ -1158,7 +1158,7 @@
         <v>36615</v>
       </c>
       <c r="B90" t="n">
-        <v>6.5</v>
+        <v>6.499999999999999</v>
       </c>
     </row>
     <row r="91">
@@ -1198,7 +1198,7 @@
         <v>36620</v>
       </c>
       <c r="B95" t="n">
-        <v>6.499999999999999</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="96">
@@ -1222,7 +1222,7 @@
         <v>36623</v>
       </c>
       <c r="B98" t="n">
-        <v>6.499999999999999</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="99">
@@ -1246,7 +1246,7 @@
         <v>36626</v>
       </c>
       <c r="B101" t="n">
-        <v>6.5</v>
+        <v>6.499999999999999</v>
       </c>
     </row>
     <row r="102">
@@ -1254,7 +1254,7 @@
         <v>36627</v>
       </c>
       <c r="B102" t="n">
-        <v>4.723855562247625</v>
+        <v>4.72393411385799</v>
       </c>
     </row>
     <row r="103">
@@ -1262,7 +1262,7 @@
         <v>36628</v>
       </c>
       <c r="B103" t="n">
-        <v>6.5</v>
+        <v>6.499999999999999</v>
       </c>
     </row>
     <row r="104">
@@ -1286,7 +1286,7 @@
         <v>36631</v>
       </c>
       <c r="B106" t="n">
-        <v>6.499999999999999</v>
+        <v>6.499999999999998</v>
       </c>
     </row>
     <row r="107">
@@ -1318,7 +1318,7 @@
         <v>36635</v>
       </c>
       <c r="B110" t="n">
-        <v>6.499999999999999</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="111">
@@ -1334,7 +1334,7 @@
         <v>36637</v>
       </c>
       <c r="B112" t="n">
-        <v>6.499999999999999</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="113">
@@ -1342,7 +1342,7 @@
         <v>36638</v>
       </c>
       <c r="B113" t="n">
-        <v>6.499999999999999</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="114">
@@ -1358,7 +1358,7 @@
         <v>36640</v>
       </c>
       <c r="B115" t="n">
-        <v>6.5</v>
+        <v>6.499999999999999</v>
       </c>
     </row>
     <row r="116">
@@ -1390,7 +1390,7 @@
         <v>36644</v>
       </c>
       <c r="B119" t="n">
-        <v>6.499999999999998</v>
+        <v>6.499999999999999</v>
       </c>
     </row>
     <row r="120">
@@ -1446,7 +1446,7 @@
         <v>36651</v>
       </c>
       <c r="B126" t="n">
-        <v>6.5</v>
+        <v>6.499999999999999</v>
       </c>
     </row>
     <row r="127">
@@ -1486,7 +1486,7 @@
         <v>36656</v>
       </c>
       <c r="B131" t="n">
-        <v>6.499999999999999</v>
+        <v>6.499999999999998</v>
       </c>
     </row>
     <row r="132">
@@ -1614,7 +1614,7 @@
         <v>36672</v>
       </c>
       <c r="B147" t="n">
-        <v>6.5</v>
+        <v>6.499999999999999</v>
       </c>
     </row>
     <row r="148">
@@ -1622,7 +1622,7 @@
         <v>36673</v>
       </c>
       <c r="B148" t="n">
-        <v>6.499999999999999</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="149">
@@ -1630,7 +1630,7 @@
         <v>36674</v>
       </c>
       <c r="B149" t="n">
-        <v>6.5</v>
+        <v>6.499999999999998</v>
       </c>
     </row>
     <row r="150">
@@ -1638,7 +1638,7 @@
         <v>36675</v>
       </c>
       <c r="B150" t="n">
-        <v>6.5</v>
+        <v>6.499999999999999</v>
       </c>
     </row>
     <row r="151">
@@ -1654,7 +1654,7 @@
         <v>36677</v>
       </c>
       <c r="B152" t="n">
-        <v>6.499999999999998</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="153">
@@ -1670,7 +1670,7 @@
         <v>36679</v>
       </c>
       <c r="B154" t="n">
-        <v>6.499999999999999</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="155">
@@ -1678,7 +1678,7 @@
         <v>36680</v>
       </c>
       <c r="B155" t="n">
-        <v>6.499999999999999</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="156">
@@ -1750,7 +1750,7 @@
         <v>36689</v>
       </c>
       <c r="B164" t="n">
-        <v>4.690109976028162</v>
+        <v>4.69029160799869</v>
       </c>
     </row>
     <row r="165">
@@ -1758,7 +1758,7 @@
         <v>36690</v>
       </c>
       <c r="B165" t="n">
-        <v>6.296566017072969</v>
+        <v>6.296751383382669</v>
       </c>
     </row>
     <row r="166">
@@ -1774,7 +1774,7 @@
         <v>36692</v>
       </c>
       <c r="B167" t="n">
-        <v>6.5</v>
+        <v>6.499999999999998</v>
       </c>
     </row>
     <row r="168">
@@ -1790,7 +1790,7 @@
         <v>36694</v>
       </c>
       <c r="B169" t="n">
-        <v>6.499999999999999</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="170">
@@ -1822,7 +1822,7 @@
         <v>36698</v>
       </c>
       <c r="B173" t="n">
-        <v>6.499999999999998</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="174">
@@ -1838,7 +1838,7 @@
         <v>36700</v>
       </c>
       <c r="B175" t="n">
-        <v>4.268082920385014</v>
+        <v>4.268272615011075</v>
       </c>
     </row>
     <row r="176">
@@ -1862,7 +1862,7 @@
         <v>36703</v>
       </c>
       <c r="B178" t="n">
-        <v>6.499999999999999</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="179">
@@ -1870,7 +1870,7 @@
         <v>36704</v>
       </c>
       <c r="B179" t="n">
-        <v>6.5</v>
+        <v>6.499999999999999</v>
       </c>
     </row>
     <row r="180">
@@ -1878,7 +1878,7 @@
         <v>36705</v>
       </c>
       <c r="B180" t="n">
-        <v>6.499999999999998</v>
+        <v>6.499999999999999</v>
       </c>
     </row>
     <row r="181">
@@ -1886,7 +1886,7 @@
         <v>36706</v>
       </c>
       <c r="B181" t="n">
-        <v>6.5</v>
+        <v>6.499999999999999</v>
       </c>
     </row>
     <row r="182">
@@ -1894,7 +1894,7 @@
         <v>36707</v>
       </c>
       <c r="B182" t="n">
-        <v>0.786748665424398</v>
+        <v>0.7867491859389353</v>
       </c>
     </row>
     <row r="183">
@@ -1902,7 +1902,7 @@
         <v>36708</v>
       </c>
       <c r="B183" t="n">
-        <v>6.499999999999998</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="184">
@@ -1918,7 +1918,7 @@
         <v>36710</v>
       </c>
       <c r="B185" t="n">
-        <v>6.499999999999998</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="186">
@@ -1926,7 +1926,7 @@
         <v>36711</v>
       </c>
       <c r="B186" t="n">
-        <v>6.499999999999998</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="187">
@@ -1950,7 +1950,7 @@
         <v>36714</v>
       </c>
       <c r="B189" t="n">
-        <v>6.499999999999998</v>
+        <v>6.499999999999999</v>
       </c>
     </row>
     <row r="190">
@@ -1974,7 +1974,7 @@
         <v>36717</v>
       </c>
       <c r="B192" t="n">
-        <v>3.100007243920883</v>
+        <v>3.099972594829565</v>
       </c>
     </row>
     <row r="193">
@@ -1982,7 +1982,7 @@
         <v>36718</v>
       </c>
       <c r="B193" t="n">
-        <v>6.5</v>
+        <v>6.499999999999999</v>
       </c>
     </row>
     <row r="194">
@@ -1990,7 +1990,7 @@
         <v>36719</v>
       </c>
       <c r="B194" t="n">
-        <v>6.499999999999999</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="195">
@@ -2038,7 +2038,7 @@
         <v>36725</v>
       </c>
       <c r="B200" t="n">
-        <v>6.499999999999999</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="201">
@@ -2054,7 +2054,7 @@
         <v>36727</v>
       </c>
       <c r="B202" t="n">
-        <v>6.5</v>
+        <v>6.499999999999998</v>
       </c>
     </row>
     <row r="203">
@@ -2134,7 +2134,7 @@
         <v>36737</v>
       </c>
       <c r="B212" t="n">
-        <v>6.5</v>
+        <v>6.499999999999999</v>
       </c>
     </row>
     <row r="213">
@@ -2174,7 +2174,7 @@
         <v>36742</v>
       </c>
       <c r="B217" t="n">
-        <v>6.5</v>
+        <v>6.499999999999999</v>
       </c>
     </row>
     <row r="218">
@@ -2190,7 +2190,7 @@
         <v>36744</v>
       </c>
       <c r="B219" t="n">
-        <v>6.499999999999999</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="220">
@@ -2198,7 +2198,7 @@
         <v>36745</v>
       </c>
       <c r="B220" t="n">
-        <v>6.5</v>
+        <v>6.499999999999999</v>
       </c>
     </row>
     <row r="221">
@@ -2206,7 +2206,7 @@
         <v>36746</v>
       </c>
       <c r="B221" t="n">
-        <v>6.5</v>
+        <v>6.499999999999998</v>
       </c>
     </row>
     <row r="222">
@@ -2238,7 +2238,7 @@
         <v>36750</v>
       </c>
       <c r="B225" t="n">
-        <v>6.5</v>
+        <v>6.499999999999999</v>
       </c>
     </row>
     <row r="226">
@@ -2254,7 +2254,7 @@
         <v>36752</v>
       </c>
       <c r="B227" t="n">
-        <v>6.499999999999999</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="228">
@@ -2270,7 +2270,7 @@
         <v>36754</v>
       </c>
       <c r="B229" t="n">
-        <v>6.499999999999999</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="230">
@@ -2302,7 +2302,7 @@
         <v>36758</v>
       </c>
       <c r="B233" t="n">
-        <v>0.7058389229682076</v>
+        <v>0.7058538671941408</v>
       </c>
     </row>
     <row r="234">
@@ -2374,7 +2374,7 @@
         <v>36767</v>
       </c>
       <c r="B242" t="n">
-        <v>6.5</v>
+        <v>6.499999999999997</v>
       </c>
     </row>
     <row r="243">
@@ -2406,7 +2406,7 @@
         <v>36771</v>
       </c>
       <c r="B246" t="n">
-        <v>6.5</v>
+        <v>6.499999999999999</v>
       </c>
     </row>
     <row r="247">
@@ -2414,7 +2414,7 @@
         <v>36772</v>
       </c>
       <c r="B247" t="n">
-        <v>6.229902054677925</v>
+        <v>6.229902799129528</v>
       </c>
     </row>
     <row r="248">
@@ -2430,7 +2430,7 @@
         <v>36774</v>
       </c>
       <c r="B249" t="n">
-        <v>6.5</v>
+        <v>6.499999999999999</v>
       </c>
     </row>
     <row r="250">
@@ -2438,7 +2438,7 @@
         <v>36775</v>
       </c>
       <c r="B250" t="n">
-        <v>6.499999999999998</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="251">
@@ -2478,7 +2478,7 @@
         <v>36780</v>
       </c>
       <c r="B255" t="n">
-        <v>6.5</v>
+        <v>6.499999999999999</v>
       </c>
     </row>
     <row r="256">
@@ -2510,7 +2510,7 @@
         <v>36784</v>
       </c>
       <c r="B259" t="n">
-        <v>6.499999999999999</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="260">
@@ -2542,7 +2542,7 @@
         <v>36788</v>
       </c>
       <c r="B263" t="n">
-        <v>6.499999999999998</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="264">
@@ -2550,7 +2550,7 @@
         <v>36789</v>
       </c>
       <c r="B264" t="n">
-        <v>6.5</v>
+        <v>6.499999999999998</v>
       </c>
     </row>
     <row r="265">
@@ -2566,7 +2566,7 @@
         <v>36791</v>
       </c>
       <c r="B266" t="n">
-        <v>6.5</v>
+        <v>6.499999999999998</v>
       </c>
     </row>
     <row r="267">
@@ -2614,7 +2614,7 @@
         <v>36797</v>
       </c>
       <c r="B272" t="n">
-        <v>5.185847319396135</v>
+        <v>5.18647357844071</v>
       </c>
     </row>
     <row r="273">
@@ -2638,7 +2638,7 @@
         <v>36800</v>
       </c>
       <c r="B275" t="n">
-        <v>6.499999999999999</v>
+        <v>6.499999999999998</v>
       </c>
     </row>
     <row r="276">
@@ -2646,7 +2646,7 @@
         <v>36801</v>
       </c>
       <c r="B276" t="n">
-        <v>2.135796674888989</v>
+        <v>2.136225066639862</v>
       </c>
     </row>
     <row r="277">
@@ -2686,7 +2686,7 @@
         <v>36806</v>
       </c>
       <c r="B281" t="n">
-        <v>6.5</v>
+        <v>6.499999999999999</v>
       </c>
     </row>
     <row r="282">
@@ -2702,7 +2702,7 @@
         <v>36808</v>
       </c>
       <c r="B283" t="n">
-        <v>6.499999999999999</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="284">
@@ -2718,7 +2718,7 @@
         <v>36810</v>
       </c>
       <c r="B285" t="n">
-        <v>6.5</v>
+        <v>6.499999999999999</v>
       </c>
     </row>
     <row r="286">
@@ -2726,7 +2726,7 @@
         <v>36811</v>
       </c>
       <c r="B286" t="n">
-        <v>6.5</v>
+        <v>6.499999999999998</v>
       </c>
     </row>
     <row r="287">
@@ -2742,7 +2742,7 @@
         <v>36813</v>
       </c>
       <c r="B288" t="n">
-        <v>6.5</v>
+        <v>6.499999999999999</v>
       </c>
     </row>
     <row r="289">
@@ -2750,7 +2750,7 @@
         <v>36814</v>
       </c>
       <c r="B289" t="n">
-        <v>6.5</v>
+        <v>6.499999999999999</v>
       </c>
     </row>
     <row r="290">
@@ -2758,7 +2758,7 @@
         <v>36815</v>
       </c>
       <c r="B290" t="n">
-        <v>6.499999999999999</v>
+        <v>6.499999999999998</v>
       </c>
     </row>
     <row r="291">
@@ -2774,7 +2774,7 @@
         <v>36817</v>
       </c>
       <c r="B292" t="n">
-        <v>6.5</v>
+        <v>6.499999999999999</v>
       </c>
     </row>
     <row r="293">
@@ -2790,7 +2790,7 @@
         <v>36819</v>
       </c>
       <c r="B294" t="n">
-        <v>6.5</v>
+        <v>6.499999999999999</v>
       </c>
     </row>
     <row r="295">
@@ -2806,7 +2806,7 @@
         <v>36821</v>
       </c>
       <c r="B296" t="n">
-        <v>6.5</v>
+        <v>6.499999999999998</v>
       </c>
     </row>
     <row r="297">
@@ -2814,7 +2814,7 @@
         <v>36822</v>
       </c>
       <c r="B297" t="n">
-        <v>6.499999999999999</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="298">
@@ -2822,7 +2822,7 @@
         <v>36823</v>
       </c>
       <c r="B298" t="n">
-        <v>1.080043133289045</v>
+        <v>1.079922354428133</v>
       </c>
     </row>
     <row r="299">
@@ -2838,7 +2838,7 @@
         <v>36825</v>
       </c>
       <c r="B300" t="n">
-        <v>0.2954278117046721</v>
+        <v>0.2954329609967254</v>
       </c>
     </row>
     <row r="301">
@@ -2846,7 +2846,7 @@
         <v>36826</v>
       </c>
       <c r="B301" t="n">
-        <v>6.499999999999999</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="302">
@@ -2894,7 +2894,7 @@
         <v>36832</v>
       </c>
       <c r="B307" t="n">
-        <v>6.499999999999999</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="308">
@@ -2902,7 +2902,7 @@
         <v>36833</v>
       </c>
       <c r="B308" t="n">
-        <v>6.5</v>
+        <v>6.499999999999999</v>
       </c>
     </row>
     <row r="309">
@@ -2926,7 +2926,7 @@
         <v>36836</v>
       </c>
       <c r="B311" t="n">
-        <v>6.499999999999999</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="312">
@@ -2934,7 +2934,7 @@
         <v>36837</v>
       </c>
       <c r="B312" t="n">
-        <v>0.5655535481938225</v>
+        <v>0.5649935200846222</v>
       </c>
     </row>
     <row r="313">
@@ -2950,7 +2950,7 @@
         <v>36839</v>
       </c>
       <c r="B314" t="n">
-        <v>6.5</v>
+        <v>6.499999999999999</v>
       </c>
     </row>
     <row r="315">
@@ -2958,7 +2958,7 @@
         <v>36840</v>
       </c>
       <c r="B315" t="n">
-        <v>0.12609768435889</v>
+        <v>0.1261379158801073</v>
       </c>
     </row>
     <row r="316">
@@ -2966,7 +2966,7 @@
         <v>36841</v>
       </c>
       <c r="B316" t="n">
-        <v>2.894319074518304</v>
+        <v>2.893638743036341</v>
       </c>
     </row>
     <row r="317">
@@ -3014,7 +3014,7 @@
         <v>36847</v>
       </c>
       <c r="B322" t="n">
-        <v>6.5</v>
+        <v>6.499999999999999</v>
       </c>
     </row>
     <row r="323">
@@ -3030,7 +3030,7 @@
         <v>36849</v>
       </c>
       <c r="B324" t="n">
-        <v>2.517149985184387</v>
+        <v>2.517950806855025</v>
       </c>
     </row>
     <row r="325">
@@ -3046,7 +3046,7 @@
         <v>36851</v>
       </c>
       <c r="B326" t="n">
-        <v>1.49527531128339</v>
+        <v>1.495255541802358</v>
       </c>
     </row>
     <row r="327">
@@ -3094,7 +3094,7 @@
         <v>36857</v>
       </c>
       <c r="B332" t="n">
-        <v>0.6121750266314212</v>
+        <v>0.6121332598989789</v>
       </c>
     </row>
     <row r="333">
@@ -3118,7 +3118,7 @@
         <v>36860</v>
       </c>
       <c r="B335" t="n">
-        <v>1.62493110558813</v>
+        <v>1.624900315127488</v>
       </c>
     </row>
     <row r="336">
@@ -3126,7 +3126,7 @@
         <v>36861</v>
       </c>
       <c r="B336" t="n">
-        <v>1.414834120556524</v>
+        <v>1.414514450828</v>
       </c>
     </row>
     <row r="337">
@@ -3142,7 +3142,7 @@
         <v>36863</v>
       </c>
       <c r="B338" t="n">
-        <v>1.311996301264805</v>
+        <v>1.311938891107031</v>
       </c>
     </row>
     <row r="339">
@@ -3150,7 +3150,7 @@
         <v>36864</v>
       </c>
       <c r="B339" t="n">
-        <v>5.458158412429904</v>
+        <v>5.457503252430285</v>
       </c>
     </row>
     <row r="340">
@@ -3158,7 +3158,7 @@
         <v>36865</v>
       </c>
       <c r="B340" t="n">
-        <v>0.6775531717677326</v>
+        <v>0.6774912530848223</v>
       </c>
     </row>
     <row r="341">
@@ -3190,7 +3190,7 @@
         <v>36869</v>
       </c>
       <c r="B344" t="n">
-        <v>0.2553614255186135</v>
+        <v>0.2554484366547911</v>
       </c>
     </row>
     <row r="345">
@@ -3206,7 +3206,7 @@
         <v>36871</v>
       </c>
       <c r="B346" t="n">
-        <v>6.374257854778179</v>
+        <v>6.373802938066352</v>
       </c>
     </row>
     <row r="347">
@@ -3214,7 +3214,7 @@
         <v>36872</v>
       </c>
       <c r="B347" t="n">
-        <v>0.8837286509344005</v>
+        <v>0.8836384728745603</v>
       </c>
     </row>
     <row r="348">
@@ -3222,7 +3222,7 @@
         <v>36873</v>
       </c>
       <c r="B348" t="n">
-        <v>5.851718010260764</v>
+        <v>5.851808341956299</v>
       </c>
     </row>
     <row r="349">
@@ -3230,7 +3230,7 @@
         <v>36874</v>
       </c>
       <c r="B349" t="n">
-        <v>0.1890045175280796</v>
+        <v>0.1890014943191278</v>
       </c>
     </row>
     <row r="350">
@@ -3238,7 +3238,7 @@
         <v>36875</v>
       </c>
       <c r="B350" t="n">
-        <v>0.1673648520848169</v>
+        <v>0.1674215479693945</v>
       </c>
     </row>
     <row r="351">
@@ -3246,7 +3246,7 @@
         <v>36876</v>
       </c>
       <c r="B351" t="n">
-        <v>0.5701308309052584</v>
+        <v>0.5700562775760289</v>
       </c>
     </row>
     <row r="352">
@@ -3254,7 +3254,7 @@
         <v>36877</v>
       </c>
       <c r="B352" t="n">
-        <v>1.119553404280457</v>
+        <v>1.119989480329731</v>
       </c>
     </row>
     <row r="353">
@@ -3262,7 +3262,7 @@
         <v>36878</v>
       </c>
       <c r="B353" t="n">
-        <v>6.5</v>
+        <v>6.499999999999999</v>
       </c>
     </row>
     <row r="354">
@@ -3294,7 +3294,7 @@
         <v>36882</v>
       </c>
       <c r="B357" t="n">
-        <v>0.8823503182300594</v>
+        <v>0.8823698774254276</v>
       </c>
     </row>
     <row r="358">
@@ -3310,7 +3310,7 @@
         <v>36884</v>
       </c>
       <c r="B359" t="n">
-        <v>4.207756353309422</v>
+        <v>4.208896489910449</v>
       </c>
     </row>
     <row r="360">
@@ -3318,7 +3318,7 @@
         <v>36885</v>
       </c>
       <c r="B360" t="n">
-        <v>5.176431865414199</v>
+        <v>5.177317777931807</v>
       </c>
     </row>
     <row r="361">
@@ -3326,7 +3326,7 @@
         <v>36886</v>
       </c>
       <c r="B361" t="n">
-        <v>6.5</v>
+        <v>6.499999999999999</v>
       </c>
     </row>
     <row r="362">
@@ -3334,7 +3334,7 @@
         <v>36887</v>
       </c>
       <c r="B362" t="n">
-        <v>4.381677948207789</v>
+        <v>4.381479864277414</v>
       </c>
     </row>
     <row r="363">
@@ -3358,7 +3358,7 @@
         <v>36890</v>
       </c>
       <c r="B365" t="n">
-        <v>0.1210389118372895</v>
+        <v>0.1210095868742612</v>
       </c>
     </row>
     <row r="366">

</xml_diff>